<commit_message>
Upload Kegiatan Praktikum Model CNN
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SEMESTER 7\MachineLearning\Praktikum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SEMESTER 7\MachineLearning\Praktikum\TugasPraktikum_120-255\PRAKTIKUM_ML_120-255\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FCEC9A4-44DC-4A12-A5CC-ECEA36F384B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9171211A-009F-45E9-8B97-0FC9F830267C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{775F54FE-02DB-4E5D-AF7E-C5C444D100D1}"/>
   </bookViews>
@@ -158,15 +158,15 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,7 +484,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,156 +497,156 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>44492</v>
       </c>
-      <c r="C3" s="5">
-        <v>44496</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="4">
+        <v>44497</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="5">
-        <v>44492</v>
-      </c>
-      <c r="C4" s="5">
-        <v>44496</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="B4" s="4">
+        <v>44497</v>
+      </c>
+      <c r="C4" s="4">
+        <v>44500</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>